<commit_message>
Final changes to Tone.cpp Initial changes to HardwareSerial.cpp
</commit_message>
<xml_diff>
--- a/EnergiaCore.xlsx
+++ b/EnergiaCore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="115">
   <si>
     <t>File</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Stream.h</t>
   </si>
   <si>
-    <t>TimerSerial.cpp</t>
-  </si>
-  <si>
-    <t>TimerSerial.h</t>
-  </si>
-  <si>
     <t>Tone.cpp</t>
   </si>
   <si>
@@ -364,6 +358,9 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>Need to determine clock cycles</t>
   </si>
 </sst>
 </file>
@@ -705,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,15 +724,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -743,7 +740,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -751,7 +748,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -769,12 +766,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -782,7 +779,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -790,7 +787,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -798,7 +795,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -806,7 +803,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -814,7 +811,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -822,7 +819,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -830,7 +827,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -838,7 +835,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -846,163 +843,158 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>39</v>
-      </c>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="D31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1014,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,10 +1021,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1040,43 +1032,43 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,44 +1077,44 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,111 +1124,115 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,24 +1242,24 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1273,88 +1269,88 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1364,28 +1360,28 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,22 +1391,22 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,175 +1416,175 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Initial write of code that has been compiled successfully -Functionality not yet tested
</commit_message>
<xml_diff>
--- a/EnergiaCore.xlsx
+++ b/EnergiaCore.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="108">
   <si>
     <t>File</t>
   </si>
@@ -75,24 +75,6 @@
     <t>Tone.cpp</t>
   </si>
   <si>
-    <t>twi.c</t>
-  </si>
-  <si>
-    <t>twi.h</t>
-  </si>
-  <si>
-    <t>usci_isr_handler.c</t>
-  </si>
-  <si>
-    <t>usci_isr_handler.h</t>
-  </si>
-  <si>
-    <t>Wire.cpp</t>
-  </si>
-  <si>
-    <t>Wire.h</t>
-  </si>
-  <si>
     <t>Wiring.c</t>
   </si>
   <si>
@@ -355,9 +337,6 @@
   </si>
   <si>
     <t>Note:need to determine overhead from function call and return</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>Need to determine clock cycles</t>
@@ -702,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,15 +703,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -740,38 +719,40 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -779,7 +760,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -787,7 +768,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -795,7 +776,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -803,7 +784,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -811,7 +792,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -819,7 +800,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -827,7 +808,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -835,7 +816,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -843,7 +824,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -851,58 +832,65 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,6 +898,9 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -918,83 +909,33 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1007,7 +948,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,10 +962,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1032,43 +973,43 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1077,44 +1018,44 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,115 +1065,115 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,24 +1183,28 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,88 +1214,88 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,28 +1305,28 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1391,22 +1336,22 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,175 +1361,207 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D40" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D43" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D45" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D46" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D47" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="C50" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E51" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D52" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="C53" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D53" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>